<commit_message>
add global map method
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OLeg\3curs\OSI\Lab4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4EDF27-23E3-4FD3-B7E8-A2C8C6134EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F9B459-DA45-4F16-B008-3D547EA7D759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="1728" windowWidth="17280" windowHeight="9420" xr2:uid="{1E596FD6-2911-4ECD-83BA-11BEFC56136A}"/>
+    <workbookView xWindow="5676" yWindow="1200" windowWidth="17280" windowHeight="9420" xr2:uid="{1E596FD6-2911-4ECD-83BA-11BEFC56136A}"/>
   </bookViews>
   <sheets>
     <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Commit</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>added parameter tuning</t>
+  </si>
+  <si>
+    <t>global map method</t>
   </si>
 </sst>
 </file>
@@ -404,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A80B89C-8FBE-4571-B251-26113691B065}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="87" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="87" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,7 +629,7 @@
         <v>11</v>
       </c>
       <c r="E14">
-        <f>C14-D14</f>
+        <f>ABS(C14-D14)</f>
         <v>1</v>
       </c>
     </row>
@@ -641,8 +644,8 @@
         <v>16</v>
       </c>
       <c r="E15">
-        <f t="shared" ref="E15:E23" si="2">C15-D15</f>
-        <v>-4</v>
+        <f t="shared" ref="E15:E23" si="2">ABS(C15-D15)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -657,7 +660,7 @@
       </c>
       <c r="E16">
         <f t="shared" si="2"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -672,7 +675,7 @@
       </c>
       <c r="E17">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -687,7 +690,7 @@
       </c>
       <c r="E18">
         <f t="shared" si="2"/>
-        <v>-4</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -717,7 +720,7 @@
       </c>
       <c r="E20">
         <f t="shared" si="2"/>
-        <v>-10</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -732,7 +735,7 @@
       </c>
       <c r="E21">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -747,7 +750,7 @@
       </c>
       <c r="E22">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -762,7 +765,7 @@
       </c>
       <c r="E23">
         <f t="shared" si="2"/>
-        <v>-5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -774,16 +777,187 @@
         <v>190</v>
       </c>
       <c r="D24">
-        <f t="shared" ref="D24:E24" si="3">SUM(D14:D23)</f>
+        <f t="shared" ref="D24" si="3">SUM(D14:D23)</f>
         <v>215</v>
       </c>
       <c r="E24">
         <f>SUM(E14:E23)</f>
-        <v>-25</v>
+        <v>31</v>
       </c>
       <c r="G24">
         <f>C24/D24</f>
         <v>0.88372093023255816</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>11</v>
+      </c>
+      <c r="D26">
+        <v>11</v>
+      </c>
+      <c r="E26">
+        <f>ABS(C26-D26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>16</v>
+      </c>
+      <c r="D27">
+        <v>16</v>
+      </c>
+      <c r="E27">
+        <f t="shared" ref="E27:E35" si="4">ABS(C27-D27)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>20</v>
+      </c>
+      <c r="D28">
+        <v>16</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+      <c r="D29">
+        <v>11</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>15</v>
+      </c>
+      <c r="D30">
+        <v>14</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>19</v>
+      </c>
+      <c r="D31">
+        <v>19</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>6</v>
+      </c>
+      <c r="C32">
+        <v>27</v>
+      </c>
+      <c r="D32">
+        <v>28</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>7</v>
+      </c>
+      <c r="C33">
+        <v>33</v>
+      </c>
+      <c r="D33">
+        <v>33</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>33</v>
+      </c>
+      <c r="D34">
+        <v>33</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>9</v>
+      </c>
+      <c r="C35">
+        <v>32</v>
+      </c>
+      <c r="D35">
+        <v>33</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <f>SUM(C26:C35)</f>
+        <v>218</v>
+      </c>
+      <c r="D36">
+        <f t="shared" ref="D36" si="5">SUM(D26:D35)</f>
+        <v>214</v>
+      </c>
+      <c r="E36">
+        <f>SUM(E26:E35)</f>
+        <v>8</v>
+      </c>
+      <c r="G36">
+        <f>C36/D36</f>
+        <v>1.0186915887850467</v>
       </c>
     </row>
   </sheetData>

</xml_diff>